<commit_message>
Adding TesNg Priority practice test
</commit_message>
<xml_diff>
--- a/SeleniumRevision/Excel/AssignData.xlsx
+++ b/SeleniumRevision/Excel/AssignData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="15960" windowHeight="6495"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="16365" windowHeight="4035"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="5">
   <si>
     <t>automationuser1983@gmail.com</t>
   </si>
@@ -373,7 +373,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -391,8 +391,8 @@
       </c>
     </row>
     <row r="2" spans="1:2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>0</v>
+      <c r="A2">
+        <v>12345.258</v>
       </c>
       <c r="B2" t="s">
         <v>2</v>

</xml_diff>